<commit_message>
(#72) Avoid error if expiration date is Unbegrenzt
</commit_message>
<xml_diff>
--- a/test/data/xlsx/Erweiterte_Arzneimittelliste_HAM_31012019.xlsx
+++ b/test/data/xlsx/Erweiterte_Arzneimittelliste_HAM_31012019.xlsx
@@ -14,6 +14,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Erweiterte Liste HAM'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Erweiterte Liste HAM'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'Erweiterte Liste HAM'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Erweiterte Liste HAM'!$7:$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'Erweiterte Liste HAM'!$7:$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'erweiterte liste ham'!#ref!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="97">
   <si>
     <t xml:space="preserve">Erweiterte Liste zugelassene Humanarzneimittel</t>
   </si>
@@ -297,7 +299,7 @@
     <t xml:space="preserve">26.04.2010</t>
   </si>
   <si>
-    <t xml:space="preserve">25.04.2020</t>
+    <t xml:space="preserve">Unbegrenzt</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
@@ -365,9 +367,6 @@
     <t xml:space="preserve">28.01.2002</t>
   </si>
   <si>
-    <t xml:space="preserve">31.08.2021</t>
-  </si>
-  <si>
     <t xml:space="preserve">immunoglobulinum humanum normale, hepatitidis B viri antigenum</t>
   </si>
   <si>
@@ -390,9 +389,6 @@
   </si>
   <si>
     <t xml:space="preserve">01.01.2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28.02.2022</t>
   </si>
   <si>
     <t xml:space="preserve">immunoglobulinum humanum normale</t>
@@ -444,9 +440,6 @@
     <t xml:space="preserve">05.07.2013</t>
   </si>
   <si>
-    <t xml:space="preserve">31.01.2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">immunoglobulinum humanum normale, immunoglobulinum humanum cytomegalicum</t>
   </si>
   <si>
@@ -474,9 +467,6 @@
     <t xml:space="preserve">30.11.1983</t>
   </si>
   <si>
-    <t xml:space="preserve">30.09.2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">polysaccharida</t>
   </si>
   <si>
@@ -496,9 +486,6 @@
   </si>
   <si>
     <t xml:space="preserve">27.09.1984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30.09.2021</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -878,18 +865,62 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF000000"/>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="General"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF9900"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <border diagonalUp="false" diagonalDown="false">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <diagonal/>
+      </border>
+      <protection locked="true" hidden="false"/>
     </dxf>
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <color rgb="FF000000"/>
+        <u val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="General"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF9900"/>
+          <bgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <border diagonalUp="false" diagonalDown="false">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <diagonal/>
+      </border>
+      <protection locked="true" hidden="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -966,9 +997,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>504360</xdr:colOff>
+      <xdr:colOff>503640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>27360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -982,7 +1013,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="85680" y="0"/>
-          <a:ext cx="1688040" cy="561240"/>
+          <a:ext cx="1687320" cy="560520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1033,15 +1064,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W65536"/>
+  <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="L8" activeCellId="0" sqref="L8:L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.4"/>
@@ -1282,7 +1313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" s="40" customFormat="true" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="40" customFormat="true" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="n">
         <v>277</v>
       </c>
@@ -1339,7 +1370,7 @@
       <c r="V8" s="32"/>
       <c r="W8" s="39"/>
     </row>
-    <row r="9" s="40" customFormat="true" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="40" customFormat="true" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="n">
         <v>278</v>
       </c>
@@ -1396,7 +1427,7 @@
       <c r="V9" s="32"/>
       <c r="W9" s="39"/>
     </row>
-    <row r="10" s="40" customFormat="true" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="40" customFormat="true" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="n">
         <v>279</v>
       </c>
@@ -1453,7 +1484,7 @@
       <c r="V10" s="32"/>
       <c r="W10" s="39"/>
     </row>
-    <row r="11" s="40" customFormat="true" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="40" customFormat="true" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="n">
         <v>282</v>
       </c>
@@ -1510,7 +1541,7 @@
       <c r="V11" s="32"/>
       <c r="W11" s="39"/>
     </row>
-    <row r="12" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="n">
         <v>488</v>
       </c>
@@ -1543,7 +1574,7 @@
         <v>55</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="M12" s="36" t="s">
         <v>35</v>
@@ -1552,14 +1583,14 @@
         <v>35</v>
       </c>
       <c r="O12" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="P12" s="37" t="s">
         <v>57</v>
-      </c>
-      <c r="P12" s="37" t="s">
-        <v>58</v>
       </c>
       <c r="Q12" s="32"/>
       <c r="R12" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S12" s="31"/>
       <c r="T12" s="32"/>
@@ -1567,7 +1598,7 @@
       <c r="V12" s="32"/>
       <c r="W12" s="39"/>
     </row>
-    <row r="13" customFormat="false" ht="250.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="241.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="n">
         <v>500</v>
       </c>
@@ -1575,13 +1606,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="E13" s="32" t="s">
         <v>61</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>62</v>
       </c>
       <c r="F13" s="31" t="s">
         <v>51</v>
@@ -1591,16 +1622,16 @@
         <v>52</v>
       </c>
       <c r="I13" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="33" t="s">
-        <v>64</v>
-      </c>
       <c r="K13" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="M13" s="36" t="s">
         <v>35</v>
@@ -1609,14 +1640,14 @@
         <v>35</v>
       </c>
       <c r="O13" s="37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P13" s="37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q13" s="32"/>
       <c r="R13" s="38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S13" s="31"/>
       <c r="T13" s="32"/>
@@ -1624,7 +1655,7 @@
       <c r="V13" s="32"/>
       <c r="W13" s="39"/>
     </row>
-    <row r="14" customFormat="false" ht="250.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="241.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="n">
         <v>500</v>
       </c>
@@ -1632,13 +1663,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="32" t="s">
         <v>61</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>62</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>51</v>
@@ -1648,16 +1679,16 @@
         <v>52</v>
       </c>
       <c r="I14" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="J14" s="33" t="s">
-        <v>64</v>
-      </c>
       <c r="K14" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L14" s="35" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="M14" s="36" t="s">
         <v>35</v>
@@ -1666,14 +1697,14 @@
         <v>35</v>
       </c>
       <c r="O14" s="37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P14" s="37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q14" s="32"/>
       <c r="R14" s="38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S14" s="31"/>
       <c r="T14" s="32"/>
@@ -1681,7 +1712,7 @@
       <c r="V14" s="32"/>
       <c r="W14" s="39"/>
     </row>
-    <row r="15" customFormat="false" ht="250.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="241.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="n">
         <v>500</v>
       </c>
@@ -1689,10 +1720,10 @@
         <v>6</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="32" t="s">
         <v>29</v>
@@ -1705,16 +1736,16 @@
         <v>52</v>
       </c>
       <c r="I15" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="33" t="s">
-        <v>64</v>
-      </c>
       <c r="K15" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L15" s="35" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="M15" s="36" t="s">
         <v>35</v>
@@ -1723,14 +1754,14 @@
         <v>35</v>
       </c>
       <c r="O15" s="37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P15" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q15" s="32"/>
       <c r="R15" s="38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S15" s="31"/>
       <c r="T15" s="32"/>
@@ -1738,7 +1769,7 @@
       <c r="V15" s="32"/>
       <c r="W15" s="39"/>
     </row>
-    <row r="16" customFormat="false" ht="250.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="241.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="n">
         <v>500</v>
       </c>
@@ -1746,13 +1777,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D16" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="32" t="s">
         <v>61</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>62</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>51</v>
@@ -1762,16 +1793,16 @@
         <v>52</v>
       </c>
       <c r="I16" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="33" t="s">
-        <v>64</v>
-      </c>
       <c r="K16" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L16" s="35" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="M16" s="36" t="s">
         <v>35</v>
@@ -1780,14 +1811,14 @@
         <v>35</v>
       </c>
       <c r="O16" s="37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P16" s="37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q16" s="32"/>
       <c r="R16" s="38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S16" s="31"/>
       <c r="T16" s="32"/>
@@ -1795,7 +1826,7 @@
       <c r="V16" s="32"/>
       <c r="W16" s="39"/>
     </row>
-    <row r="17" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29" t="n">
         <v>506</v>
       </c>
@@ -1803,7 +1834,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>50</v>
@@ -1819,16 +1850,16 @@
         <v>52</v>
       </c>
       <c r="I17" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J17" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="K17" s="34" t="s">
-        <v>78</v>
-      </c>
       <c r="L17" s="35" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="M17" s="36" t="s">
         <v>35</v>
@@ -1837,14 +1868,14 @@
         <v>35</v>
       </c>
       <c r="O17" s="37" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="P17" s="37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q17" s="32"/>
       <c r="R17" s="38" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="S17" s="31"/>
       <c r="T17" s="32"/>
@@ -1852,7 +1883,7 @@
       <c r="V17" s="32"/>
       <c r="W17" s="39"/>
     </row>
-    <row r="18" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="n">
         <v>509</v>
       </c>
@@ -1860,32 +1891,32 @@
         <v>1</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E18" s="32" t="s">
         <v>29</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G18" s="31"/>
       <c r="H18" s="32" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I18" s="32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J18" s="33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L18" s="35" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="M18" s="36" t="s">
         <v>35</v>
@@ -1894,14 +1925,14 @@
         <v>35</v>
       </c>
       <c r="O18" s="37" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="P18" s="37" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Q18" s="32"/>
       <c r="R18" s="38" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="S18" s="31"/>
       <c r="T18" s="32"/>
@@ -1909,7 +1940,7 @@
       <c r="V18" s="32"/>
       <c r="W18" s="39"/>
     </row>
-    <row r="19" customFormat="false" ht="91.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="n">
         <v>520</v>
       </c>
@@ -1917,48 +1948,48 @@
         <v>1</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E19" s="32" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G19" s="31"/>
       <c r="H19" s="32" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I19" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="K19" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="L19" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="N19" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="O19" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="P19" s="37" t="s">
         <v>95</v>
-      </c>
-      <c r="J19" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="K19" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="L19" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="M19" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="N19" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="O19" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="P19" s="37" t="s">
-        <v>100</v>
       </c>
       <c r="Q19" s="32"/>
       <c r="R19" s="38" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="S19" s="31"/>
       <c r="T19" s="32"/>

</xml_diff>